<commit_message>
Fix issues #351 and #352
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41638506-3671-4BAB-A4CE-9AF7C32F10D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B29FEA-E98A-4AC6-B82D-4673DB73DB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>group</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>yScaleFactors</t>
+  </si>
+  <si>
+    <t>name</t>
   </si>
 </sst>
 </file>
@@ -490,7 +493,7 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -649,19 +652,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>19</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fix "error" to "stop" Update to RoxygenNote: 7.2.2 Exit early if no DataCombined is defined
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B29FEA-E98A-4AC6-B82D-4673DB73DB2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06B440-D073-4F32-8AAE-6A2D29C4C634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
   <si>
     <t>group</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>name</t>
+  </si>
+  <si>
+    <t>AciclovirPVB</t>
   </si>
 </sst>
 </file>
@@ -178,7 +181,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -194,7 +197,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -493,22 +496,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.46875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.3515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.46875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.3515625" customWidth="1"/>
-    <col min="6" max="6" width="77.64453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -543,7 +546,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
       <c r="B2"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
@@ -579,22 +585,22 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.52734375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.05859375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.8203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.46875" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.8203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.17578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.234375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.17578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -654,11 +660,11 @@
   <sheetPr codeName="Tabelle3"/>
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -683,19 +689,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.64453125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -714,34 +720,34 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -752,26 +758,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -974,26 +960,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1010,4 +997,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Throw an error if no path is provided for a simulation result
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E06B440-D073-4F32-8AAE-6A2D29C4C634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF95E19-31CB-4F52-A300-7A61341F8413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
   <si>
     <t>group</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>AciclovirPVB</t>
+  </si>
+  <si>
+    <t>Aciclovir simulated</t>
+  </si>
+  <si>
+    <t>TestScenario</t>
   </si>
 </sst>
 </file>
@@ -497,7 +503,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,8 +556,15 @@
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2"/>
-      <c r="D2" s="3"/>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E2" s="3"/>
       <c r="F2" s="2"/>
     </row>
@@ -568,7 +581,7 @@
           <x14:formula1>
             <xm:f>dataTypes!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>B2 B3:B1048576</xm:sqref>
+          <xm:sqref>B2:B1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Do not fail if no data transformations are specified
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDF95E19-31CB-4F52-A300-7A61341F8413}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8316C9F2-3E70-41B5-B9A9-AF3FCC50C845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>group</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>TestScenario</t>
+  </si>
+  <si>
+    <t>Organism|PeripheralVenousBlood|Aciclovir|Plasma (Peripheral Venous Blood)</t>
   </si>
 </sst>
 </file>
@@ -503,7 +506,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -565,7 +568,9 @@
       <c r="D2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="3"/>
+      <c r="E2" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="F2" s="2"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Code refactor Error checks Tests Updated Plots.xlsx
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8316C9F2-3E70-41B5-B9A9-AF3FCC50C845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF27A0D-A092-4313-B8A7-0D4662AAF956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>group</t>
   </si>
@@ -144,6 +144,36 @@
   </si>
   <si>
     <t>Organism|PeripheralVenousBlood|Aciclovir|Plasma (Peripheral Venous Blood)</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>Aciclovri observed</t>
+  </si>
+  <si>
+    <t>Aciclovir_Laskin 1982.Group A_1_Human_PeripheralVenousBlood_Plasma_2.5 mg/kg_iv</t>
+  </si>
+  <si>
+    <t>Aciclovir</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P1, P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>Aciclovr2</t>
+  </si>
+  <si>
+    <t>blabla</t>
+  </si>
+  <si>
+    <t>1;2;3</t>
   </si>
 </sst>
 </file>
@@ -179,7 +209,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -187,7 +217,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -503,10 +532,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF424A-768A-416F-94F0-2A05F47DDD9E}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,7 +544,7 @@
     <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
@@ -565,13 +594,30 @@
       <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" t="s">
         <v>33</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" t="s">
         <v>34</v>
       </c>
       <c r="F2" s="2"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -597,10 +643,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,7 +664,7 @@
     <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -654,6 +700,45 @@
       </c>
       <c r="L1" t="s">
         <v>14</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="N2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -676,9 +761,11 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -691,6 +778,22 @@
       </c>
       <c r="C1" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B3" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -735,7 +838,7 @@
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,6 +879,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -978,17 +1092,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -999,6 +1102,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1017,17 +1131,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix #353. Support additional parameters for plotConfiguration and exportConfiguration, not yet plotGrids (#354)
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF27A0D-A092-4313-B8A7-0D4662AAF956}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C92E2B-AAD4-4790-AD47-3C5ADF21B470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="9027" yWindow="2167" windowWidth="13373" windowHeight="10073" firstSheet="1" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
     <sheet name="plotConfiguration" sheetId="9" r:id="rId2"/>
     <sheet name="plotGrids" sheetId="5" r:id="rId3"/>
-    <sheet name="dataTypes" sheetId="4" r:id="rId4"/>
-    <sheet name="plotTypes" sheetId="10" r:id="rId5"/>
+    <sheet name="exportConfiguration" sheetId="11" r:id="rId4"/>
+    <sheet name="dataTypes" sheetId="4" r:id="rId5"/>
+    <sheet name="plotTypes" sheetId="10" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
   <si>
     <t>group</t>
   </si>
@@ -174,6 +175,21 @@
   </si>
   <si>
     <t>1;2;3</t>
+  </si>
+  <si>
+    <t>plotGridName</t>
+  </si>
+  <si>
+    <t>outputName</t>
+  </si>
+  <si>
+    <t>Aciclovir1</t>
+  </si>
+  <si>
+    <t>width</t>
+  </si>
+  <si>
+    <t>Aciclovir2</t>
   </si>
 </sst>
 </file>
@@ -219,7 +235,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -235,7 +251,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -523,7 +539,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -534,22 +550,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="F1" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -584,7 +600,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -602,7 +618,7 @@
       </c>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -616,7 +632,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -645,26 +661,26 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.87890625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1171875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.29296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1171875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.29296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -705,7 +721,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -719,7 +735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -730,7 +746,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -764,12 +780,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -780,7 +796,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -788,7 +804,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -802,6 +818,51 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C15D6C-2CD2-47AE-90A6-7EE546C5950C}">
   <sheetPr codeName="Tabelle4"/>
   <dimension ref="A1:A3"/>
@@ -810,19 +871,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -832,7 +893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8551BE5-7C15-4718-88B4-27F1A938F9CF}">
   <sheetPr codeName="Tabelle5"/>
   <dimension ref="A1:A6"/>
@@ -841,34 +902,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -879,17 +940,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1092,6 +1142,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1102,17 +1163,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1131,6 +1181,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
-Add check if the property defined in the excel file is supported by the configuration object
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C92E2B-AAD4-4790-AD47-3C5ADF21B470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5680D-6869-4942-8669-79907222D007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9027" yWindow="2167" windowWidth="13373" windowHeight="10073" firstSheet="1" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>group</t>
   </si>
@@ -171,12 +171,6 @@
     <t>Aciclovr2</t>
   </si>
   <si>
-    <t>blabla</t>
-  </si>
-  <si>
-    <t>1;2;3</t>
-  </si>
-  <si>
     <t>plotGridName</t>
   </si>
   <si>
@@ -190,6 +184,9 @@
   </si>
   <si>
     <t>Aciclovir2</t>
+  </si>
+  <si>
+    <t>Aciclovir PVB</t>
   </si>
 </sst>
 </file>
@@ -235,7 +232,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -251,7 +248,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -539,7 +536,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -550,22 +547,22 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -600,7 +597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -617,8 +614,11 @@
         <v>34</v>
       </c>
       <c r="F2" s="2"/>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -631,8 +631,11 @@
       <c r="F3" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="G3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -659,28 +662,28 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.87890625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.29296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1171875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.29296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -717,11 +720,8 @@
       <c r="L1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -731,11 +731,8 @@
       <c r="C2" t="s">
         <v>21</v>
       </c>
-      <c r="N2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -746,7 +743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -780,12 +777,12 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -796,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -804,7 +801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -821,40 +818,45 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C1" t="s">
         <v>46</v>
       </c>
-      <c r="C1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>38</v>
       </c>
       <c r="B3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -871,19 +873,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -902,34 +904,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -940,6 +942,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1142,7 +1153,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -1153,16 +1164,15 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1181,7 +1191,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1190,12 +1200,4 @@
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix for the case when not all data combined objects are used in plot grids
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9A5680D-6869-4942-8669-79907222D007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC257E40-40E8-4583-BACF-38D33BDB1A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -548,21 +548,21 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>20</v>
       </c>
@@ -597,7 +597,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -618,7 +618,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -635,7 +635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -668,22 +668,22 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.1328125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -721,7 +721,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>35</v>
       </c>
@@ -732,7 +732,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>39</v>
       </c>
@@ -743,7 +743,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>41</v>
       </c>
@@ -780,9 +780,9 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>30</v>
       </c>
@@ -793,7 +793,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -801,7 +801,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>42</v>
       </c>
@@ -822,14 +822,14 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>43</v>
       </c>
@@ -840,7 +840,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -851,7 +851,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -873,19 +873,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -904,34 +904,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -942,15 +942,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1153,7 +1144,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -1164,15 +1155,16 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1191,7 +1183,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -1200,4 +1192,12 @@
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
- Only apply transformations to DataCombined that are actually used - When only one plot is in the grid, do not show panel labels - Try to get the expected type of configuration fields specified in additional excel columns - xAxisLimits and yAxisLimits are in one column now, separated by ','
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC257E40-40E8-4583-BACF-38D33BDB1A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78FF88-8984-439A-AAB1-81BD29048112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>group</t>
   </si>
@@ -75,18 +75,6 @@
     <t>dataSet</t>
   </si>
   <si>
-    <t>xLimLower</t>
-  </si>
-  <si>
-    <t>xLimUpper</t>
-  </si>
-  <si>
-    <t>yLimLower</t>
-  </si>
-  <si>
-    <t>yLimUpper</t>
-  </si>
-  <si>
     <t>plotID</t>
   </si>
   <si>
@@ -187,6 +175,15 @@
   </si>
   <si>
     <t>Aciclovir PVB</t>
+  </si>
+  <si>
+    <t>xAxisLimits</t>
+  </si>
+  <si>
+    <t>yAxisLimits</t>
+  </si>
+  <si>
+    <t>0, 24</t>
   </si>
 </sst>
 </file>
@@ -547,30 +544,30 @@
   <sheetPr codeName="Tabelle1"/>
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -585,57 +582,57 @@
         <v>0</v>
       </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>27</v>
-      </c>
-      <c r="J1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>31</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -662,33 +659,30 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.265625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.1328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
         <v>5</v>
@@ -703,55 +697,52 @@
         <v>4</v>
       </c>
       <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" t="s">
         <v>17</v>
       </c>
-      <c r="H1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" t="s">
-        <v>11</v>
-      </c>
-      <c r="J1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="I2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="B2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
       <c r="B3" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C4" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -780,33 +771,33 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>42</v>
-      </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -822,41 +813,41 @@
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C2">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -873,19 +864,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -904,36 +895,36 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -942,6 +933,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1144,27 +1155,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1181,23 +1191,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Remove entries from export configuration sheet as the tests are failing
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78FF88-8984-439A-AAB1-81BD29048112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F7A6E-2826-487E-9E61-232C509A485A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>group</t>
   </si>
@@ -165,13 +165,7 @@
     <t>outputName</t>
   </si>
   <si>
-    <t>Aciclovir1</t>
-  </si>
-  <si>
     <t>width</t>
-  </si>
-  <si>
-    <t>Aciclovir2</t>
   </si>
   <si>
     <t>Aciclovir PVB</t>
@@ -533,7 +527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,7 +606,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -629,7 +623,7 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -661,7 +655,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -703,10 +697,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -720,7 +714,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -807,9 +801,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
@@ -828,26 +822,7 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
         <v>41</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -933,15 +908,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -950,6 +916,15 @@
     <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1156,20 +1131,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Add argument `plotGridNames` that allow specification of which plots … (#377)
* Add argument `plotGridNames` that allow specification of which plots to create

* Return missing test
Styler
Update documentation

* Remove entries from export configuration sheet as the tests are failing
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E78FF88-8984-439A-AAB1-81BD29048112}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F7A6E-2826-487E-9E61-232C509A485A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
   <si>
     <t>group</t>
   </si>
@@ -165,13 +165,7 @@
     <t>outputName</t>
   </si>
   <si>
-    <t>Aciclovir1</t>
-  </si>
-  <si>
     <t>width</t>
-  </si>
-  <si>
-    <t>Aciclovir2</t>
   </si>
   <si>
     <t>Aciclovir PVB</t>
@@ -533,7 +527,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,7 +606,7 @@
       </c>
       <c r="F2" s="2"/>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -629,7 +623,7 @@
         <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -661,7 +655,7 @@
   <sheetPr codeName="Tabelle2"/>
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
@@ -703,10 +697,10 @@
         <v>14</v>
       </c>
       <c r="I1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -720,7 +714,7 @@
         <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -807,9 +801,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
@@ -828,26 +822,7 @@
         <v>40</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
         <v>41</v>
-      </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" t="s">
-        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -933,15 +908,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
@@ -950,6 +916,15 @@
     <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1156,20 +1131,20 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
     <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Fix #354, #360, #372
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F7A6E-2826-487E-9E61-232C509A485A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AA5BA-08CB-449D-A9AF-DDE7E88152A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="2740" yWindow="1213" windowWidth="19200" windowHeight="10074" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>group</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>0, 24</t>
+  </si>
+  <si>
+    <t>quantiles</t>
+  </si>
+  <si>
+    <t>foldDistance</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>tagPrefix</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,7 +251,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,18 +554,18 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -588,7 +600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -609,7 +621,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -626,7 +638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -653,25 +665,25 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -702,8 +714,14 @@
       <c r="J1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -717,7 +735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -727,8 +745,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -759,62 +780,65 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -839,19 +863,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -870,34 +894,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -908,26 +932,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1130,26 +1134,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1166,4 +1171,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fix #354, #360, #372 (#383)
Co-authored-by: Johanna Eitel <johanna.eitel@esqlabs.com>
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A43F7A6E-2826-487E-9E61-232C509A485A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AA5BA-08CB-449D-A9AF-DDE7E88152A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19103" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="3" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="2740" yWindow="1213" windowWidth="19200" windowHeight="10074" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
   <si>
     <t>group</t>
   </si>
@@ -178,6 +178,18 @@
   </si>
   <si>
     <t>0, 24</t>
+  </si>
+  <si>
+    <t>quantiles</t>
+  </si>
+  <si>
+    <t>foldDistance</t>
+  </si>
+  <si>
+    <t>2, 3</t>
+  </si>
+  <si>
+    <t>tagPrefix</t>
   </si>
 </sst>
 </file>
@@ -223,7 +235,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -239,7 +251,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -542,18 +554,18 @@
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -588,7 +600,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -609,7 +621,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -626,7 +638,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -653,25 +665,25 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73B8908D-615D-4618-BFCF-D7DBA10892F0}">
   <sheetPr codeName="Tabelle2"/>
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="5.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.29296875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.5859375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -702,8 +714,14 @@
       <c r="J1" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>46</v>
+      </c>
+      <c r="L1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -717,7 +735,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -727,8 +745,11 @@
       <c r="C3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -759,62 +780,65 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C90A7A38-3099-4667-B241-E28D7B8B0B13}">
-  <dimension ref="A1:C1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.29296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -839,19 +863,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -870,34 +894,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -908,26 +932,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1130,26 +1134,27 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1166,4 +1171,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added columns for unit specification of x and y offsets in plots excel
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AA5BA-08CB-449D-A9AF-DDE7E88152A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F8E777-9860-477C-803A-6F9B770CF38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1213" windowWidth="19200" windowHeight="10074" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>group</t>
   </si>
@@ -189,7 +189,16 @@
     <t>2, 3</t>
   </si>
   <si>
-    <t>tagPrefix</t>
+    <t>xOffsetsUnits</t>
+  </si>
+  <si>
+    <t>yOffsetsUnits</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -235,7 +244,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -251,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -539,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,24 +557,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF424A-768A-416F-94F0-2A05F47DDD9E}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -591,16 +600,22 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -620,8 +635,14 @@
       <c r="G2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -637,8 +658,14 @@
       <c r="G3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -671,19 +698,19 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -721,7 +748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -735,7 +762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -749,7 +776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -780,15 +807,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -798,11 +825,8 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -810,7 +834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -831,14 +855,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -863,19 +887,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -894,34 +918,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -932,6 +956,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1134,27 +1178,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1171,23 +1214,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added columns for unit specification of x and y offsets in plots excel (#390)
* Added columns for unit specification of x and y offsets in plots excel

* Update R/utilities-data-combined.R

* Fix for y offsets

* Avoid using %in%
</commit_message>
<xml_diff>
--- a/tests/data/TestProject/Parameters/Plots.xlsx
+++ b/tests/data/TestProject/Parameters/Plots.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\github\esqlabsR\tests\data\TestProject\Parameters\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\OSPS\Repos\esqlabsR\tests\data\TestProject\Parameters\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095AA5BA-08CB-449D-A9AF-DDE7E88152A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F8E777-9860-477C-803A-6F9B770CF38D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2740" yWindow="1213" windowWidth="19200" windowHeight="10074" activeTab="2" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
+    <workbookView xWindow="38280" yWindow="-15" windowWidth="38640" windowHeight="21120" xr2:uid="{3D43716F-F01F-40EA-AEC2-E6E5F12B752F}"/>
   </bookViews>
   <sheets>
     <sheet name="DataCombined" sheetId="3" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="53">
   <si>
     <t>group</t>
   </si>
@@ -189,7 +189,16 @@
     <t>2, 3</t>
   </si>
   <si>
-    <t>tagPrefix</t>
+    <t>xOffsetsUnits</t>
+  </si>
+  <si>
+    <t>yOffsetsUnits</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>min</t>
   </si>
 </sst>
 </file>
@@ -235,7 +244,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -251,7 +260,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -539,7 +548,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -548,24 +557,24 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2CF424A-768A-416F-94F0-2A05F47DDD9E}">
   <sheetPr codeName="Tabelle1"/>
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.1171875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.29296875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41015625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="73.41015625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="77.703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="24.87890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.265625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="73.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.73046875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -591,16 +600,22 @@
         <v>22</v>
       </c>
       <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
         <v>23</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -620,8 +635,14 @@
       <c r="G2" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H2">
+        <v>1</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -637,8 +658,14 @@
       <c r="G3" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.5">
+      <c r="H3">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="B4"/>
     </row>
   </sheetData>
@@ -671,19 +698,19 @@
       <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="5.5859375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5859375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.41015625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.87890625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.41015625" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="10.29296875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.5859375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.86328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.3984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="10.265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>11</v>
       </c>
@@ -721,7 +748,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -735,7 +762,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -749,7 +776,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>37</v>
       </c>
@@ -780,15 +807,15 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FF3CB29-E548-4DAF-A68B-014C6C094FDA}">
   <sheetPr codeName="Tabelle3"/>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>26</v>
       </c>
@@ -798,11 +825,8 @@
       <c r="C1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.5">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -810,7 +834,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>38</v>
       </c>
@@ -831,14 +855,14 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.29296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.1171875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.73046875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.1328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -863,19 +887,19 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.703125" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="10.73046875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -894,34 +918,34 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.41015625" defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultColWidth="11.3984375" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>21</v>
       </c>
@@ -932,6 +956,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x01010011DB5BA7A27696418C6D2C8B46A68E83" ma:contentTypeVersion="12" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7db5ef2c9b694ee90a55e1e15107ca02">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="398d2b5b-77f8-4c5f-a794-3d35ce849315" xmlns:ns3="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ddfc242a629ea5bba70a4577bac7893e" ns2:_="" ns3:_="">
     <xsd:import namespace="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
@@ -1134,27 +1178,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="398d2b5b-77f8-4c5f-a794-3d35ce849315">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="1c52e43a-7a2d-43c4-9ede-f251c929c0a1" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
+    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E9CB25A-A0F7-4E2B-B2A8-1E0ACE86AF84}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1171,23 +1214,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BCC0D355-BB44-49CE-BEA9-BF722D315860}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{07DA2F2C-8C96-42F3-AA23-50DABD54D547}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="398d2b5b-77f8-4c5f-a794-3d35ce849315"/>
-    <ds:schemaRef ds:uri="1c52e43a-7a2d-43c4-9ede-f251c929c0a1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>